<commit_message>
Completed blog post #5 with images
</commit_message>
<xml_diff>
--- a/performace-testing/results/DataAnalysis.xlsx
+++ b/performace-testing/results/DataAnalysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ray-tracer-challenge-netcore\performace-testing\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simone/Documents/Projects/ray-tracer-challenge-netcore/performace-testing/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21360" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,15 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$176</definedName>
     <definedName name="MyBenchmarks.StringConcatOptions_report" localSheetId="0">Sheet1!$A$1:$D$176</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -663,7 +669,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -718,7 +724,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -792,150 +798,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$D$28:$H$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$D$26:$H$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1550</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16600</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>324200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-8168-46A9-9070-D737354538FC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$C$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>StringBuilder</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet3!$D$28:$H$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$D$27:$H$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1650</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13600</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>141300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-8168-46A9-9070-D737354538FC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$C$26</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>StringJoin</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -955,19 +817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,33 +841,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>95.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>163</c:v>
+                  <c:v>163.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1550</c:v>
+                  <c:v>1550.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16600</c:v>
+                  <c:v>16600.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>324200</c:v>
+                  <c:v>324200.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8168-46A9-9070-D737354538FC}"/>
+              <c16:uniqueId val="{00000006-8168-46A9-9070-D737354538FC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:idx val="3"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet3!$C$27</c:f>
@@ -1036,19 +898,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,27 +922,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>210</c:v>
+                  <c:v>210.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1650</c:v>
+                  <c:v>1650.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13600</c:v>
+                  <c:v>13600.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141300</c:v>
+                  <c:v>141300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-8168-46A9-9070-D737354538FC}"/>
+              <c16:uniqueId val="{00000007-8168-46A9-9070-D737354538FC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1093,11 +955,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565367568"/>
-        <c:axId val="565369208"/>
+        <c:axId val="957322880"/>
+        <c:axId val="957325712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565367568"/>
+        <c:axId val="957322880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,7 +1002,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565369208"/>
+        <c:crossAx val="957325712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1148,9 +1010,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565369208"/>
+        <c:axId val="957325712"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1200,7 +1062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565367568"/>
+        <c:crossAx val="957322880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1260,7 +1122,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1323,6 +1185,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1333,19 +1206,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,25 +1230,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>115</c:v>
+                  <c:v>115.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>213</c:v>
+                  <c:v>213.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2068</c:v>
+                  <c:v>2068.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30000</c:v>
+                  <c:v>30000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>700000</c:v>
+                  <c:v>700000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2A2B-4CBF-A738-E1DAAB14B5D0}"/>
             </c:ext>
@@ -1384,6 +1257,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringBuilder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1394,19 +1278,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,25 +1302,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>140</c:v>
+                  <c:v>140.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>374</c:v>
+                  <c:v>374.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2066</c:v>
+                  <c:v>2066.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18000</c:v>
+                  <c:v>18000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250000</c:v>
+                  <c:v>250000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2A2B-4CBF-A738-E1DAAB14B5D0}"/>
             </c:ext>
@@ -1451,11 +1335,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565367568"/>
-        <c:axId val="565369208"/>
+        <c:axId val="1032864224"/>
+        <c:axId val="1032866976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565367568"/>
+        <c:axId val="1032864224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565369208"/>
+        <c:crossAx val="1032866976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1506,9 +1390,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565369208"/>
+        <c:axId val="1032866976"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1558,7 +1442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565367568"/>
+        <c:crossAx val="1032864224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1618,7 +1502,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1700,6 +1584,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1719,25 +1614,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1749,31 +1644,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1100</c:v>
+                  <c:v>1100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1100</c:v>
+                  <c:v>1100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1270</c:v>
+                  <c:v>1270.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1370</c:v>
+                  <c:v>1370.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1550</c:v>
+                  <c:v>1550.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2068</c:v>
+                  <c:v>2068.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B0E1-42E5-8588-3B059C1E8B06}"/>
             </c:ext>
@@ -1782,6 +1677,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringBuilder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1801,25 +1707,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1831,31 +1737,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>600</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1200</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1350</c:v>
+                  <c:v>1350.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1460</c:v>
+                  <c:v>1460.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1650</c:v>
+                  <c:v>1650.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2066</c:v>
+                  <c:v>2066.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B0E1-42E5-8588-3B059C1E8B06}"/>
             </c:ext>
@@ -1870,11 +1776,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="707798480"/>
-        <c:axId val="707798808"/>
+        <c:axId val="1032891568"/>
+        <c:axId val="1032894320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="707798480"/>
+        <c:axId val="1032891568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,7 +1823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="707798808"/>
+        <c:crossAx val="1032894320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1925,7 +1831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="707798808"/>
+        <c:axId val="1032894320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="707798480"/>
+        <c:crossAx val="1032891568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2058,7 +1964,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2141,6 +2047,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringJoin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2160,25 +2077,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,31 +2107,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>111.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
+                  <c:v>114.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142</c:v>
+                  <c:v>142.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>160.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>184</c:v>
+                  <c:v>184.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>324</c:v>
+                  <c:v>324.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>710</c:v>
+                  <c:v>710.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A589-402B-B923-2008A53AF742}"/>
             </c:ext>
@@ -2223,6 +2140,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringBuilder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2242,25 +2170,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,31 +2200,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>116</c:v>
+                  <c:v>116.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>140</c:v>
+                  <c:v>140.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>251</c:v>
+                  <c:v>251.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A589-402B-B923-2008A53AF742}"/>
             </c:ext>
@@ -2311,11 +2239,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565369536"/>
-        <c:axId val="565366584"/>
+        <c:axId val="1032918800"/>
+        <c:axId val="1032921552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565369536"/>
+        <c:axId val="1032918800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2358,7 +2286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565366584"/>
+        <c:crossAx val="1032921552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2366,8 +2294,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565366584"/>
+        <c:axId val="1032921552"/>
         <c:scaling>
+          <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2417,7 +2346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565369536"/>
+        <c:crossAx val="1032918800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3614,16 +3543,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>150812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36512</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3644,16 +3573,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3676,16 +3605,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>661987</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>115887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>293687</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>1587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3706,16 +3635,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>650875</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>141287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>282575</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>26987</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4004,23 +3933,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D92" sqref="D92:D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +3963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4048,7 +3977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4062,7 +3991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4077,7 +4006,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4091,7 +4020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4105,7 +4034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4119,7 +4048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4133,7 +4062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4147,7 +4076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4161,7 +4090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4175,7 +4104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4189,7 +4118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -4203,7 +4132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -4218,7 +4147,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -4233,7 +4162,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4247,7 +4176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -4261,7 +4190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -4275,7 +4204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -4290,7 +4219,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4305,7 +4234,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4319,7 +4248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -4333,7 +4262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4347,7 +4276,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -4362,7 +4291,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -4377,7 +4306,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -4391,7 +4320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -4405,7 +4334,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -4419,7 +4348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -4434,7 +4363,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -4449,7 +4378,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -4463,7 +4392,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -4477,7 +4406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -4491,7 +4420,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -4506,7 +4435,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -4521,7 +4450,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4535,7 +4464,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -4549,7 +4478,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -4563,7 +4492,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -4577,7 +4506,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -4591,7 +4520,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4605,7 +4534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -4619,7 +4548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -4633,7 +4562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -4647,7 +4576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -4661,7 +4590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4675,7 +4604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -4689,7 +4618,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -4703,7 +4632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -4717,7 +4646,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -4731,7 +4660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -4745,7 +4674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -4759,7 +4688,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -4773,7 +4702,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -4787,7 +4716,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -4801,7 +4730,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -4815,7 +4744,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -4829,7 +4758,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -4843,7 +4772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -4857,7 +4786,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -4871,7 +4800,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -4885,7 +4814,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -4899,7 +4828,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -4913,7 +4842,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -4927,7 +4856,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -4941,7 +4870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -4955,7 +4884,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -4969,7 +4898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -4983,7 +4912,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -4997,7 +4926,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -5011,7 +4940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -5025,7 +4954,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -5039,7 +4968,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -5053,7 +4982,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -5067,7 +4996,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -5081,7 +5010,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -5095,7 +5024,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -5109,7 +5038,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -5123,7 +5052,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -5137,7 +5066,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -5151,7 +5080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -5165,7 +5094,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -5179,7 +5108,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -5193,7 +5122,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -5207,7 +5136,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -5221,7 +5150,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -5235,7 +5164,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -5249,7 +5178,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -5263,7 +5192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -5277,7 +5206,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -5291,7 +5220,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -5305,7 +5234,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -5319,7 +5248,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -5333,7 +5262,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -5347,7 +5276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -5361,7 +5290,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -5375,7 +5304,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -5389,7 +5318,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -5403,7 +5332,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -5417,7 +5346,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -5431,7 +5360,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -5445,7 +5374,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -5459,7 +5388,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -5473,7 +5402,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -5487,7 +5416,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -5501,7 +5430,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -5515,7 +5444,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -5529,7 +5458,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -5543,7 +5472,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -5557,7 +5486,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -5571,7 +5500,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -5585,7 +5514,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -5599,7 +5528,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -5613,7 +5542,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -5627,7 +5556,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -5641,7 +5570,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>12</v>
       </c>
@@ -5655,7 +5584,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>4</v>
       </c>
@@ -5669,7 +5598,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -5683,7 +5612,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -5697,7 +5626,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -5711,7 +5640,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>12</v>
       </c>
@@ -5725,7 +5654,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -5739,7 +5668,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -5753,7 +5682,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -5767,7 +5696,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -5781,7 +5710,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>12</v>
       </c>
@@ -5795,7 +5724,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>4</v>
       </c>
@@ -5809,7 +5738,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -5823,7 +5752,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -5837,7 +5766,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -5851,7 +5780,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -5865,7 +5794,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -5879,7 +5808,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -5893,7 +5822,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -5907,7 +5836,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>10</v>
       </c>
@@ -5921,7 +5850,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>12</v>
       </c>
@@ -5935,7 +5864,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>4</v>
       </c>
@@ -5949,7 +5878,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>6</v>
       </c>
@@ -5963,7 +5892,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -5977,7 +5906,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -5991,7 +5920,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -6005,7 +5934,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -6019,7 +5948,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>6</v>
       </c>
@@ -6033,7 +5962,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -6047,7 +5976,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -6061,7 +5990,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -6075,7 +6004,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>4</v>
       </c>
@@ -6089,7 +6018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -6103,7 +6032,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -6117,7 +6046,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -6131,7 +6060,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>12</v>
       </c>
@@ -6145,7 +6074,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>4</v>
       </c>
@@ -6159,7 +6088,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>6</v>
       </c>
@@ -6173,7 +6102,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -6187,7 +6116,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -6201,7 +6130,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>12</v>
       </c>
@@ -6215,7 +6144,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>4</v>
       </c>
@@ -6229,7 +6158,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>6</v>
       </c>
@@ -6243,7 +6172,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -6257,7 +6186,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -6271,7 +6200,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>12</v>
       </c>
@@ -6285,7 +6214,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>4</v>
       </c>
@@ -6299,7 +6228,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>6</v>
       </c>
@@ -6313,7 +6242,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -6327,7 +6256,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -6341,7 +6270,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>12</v>
       </c>
@@ -6355,7 +6284,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>4</v>
       </c>
@@ -6369,7 +6298,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>6</v>
       </c>
@@ -6383,7 +6312,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -6397,7 +6326,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -6411,7 +6340,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>12</v>
       </c>
@@ -6425,7 +6354,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>4</v>
       </c>
@@ -6439,7 +6368,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>6</v>
       </c>
@@ -6453,7 +6382,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -6467,7 +6396,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>10</v>
       </c>
@@ -6481,7 +6410,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>12</v>
       </c>
@@ -6518,22 +6447,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D3" s="2">
         <v>1</v>
       </c>
@@ -6556,7 +6485,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>186</v>
       </c>
@@ -6585,7 +6514,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>10</v>
       </c>
@@ -6611,7 +6540,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>100</v>
       </c>
@@ -6637,7 +6566,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>1000</v>
       </c>
@@ -6663,7 +6592,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>10000</v>
       </c>
@@ -6689,7 +6618,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -6709,7 +6638,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>8</v>
       </c>
@@ -6729,7 +6658,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>5</v>
       </c>
@@ -6746,7 +6675,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -6766,7 +6695,7 @@
         <v>324200</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>8</v>
       </c>
@@ -6786,7 +6715,7 @@
         <v>141300</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D28">
         <v>5</v>
       </c>
@@ -6803,12 +6732,12 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>4</v>
       </c>
@@ -6834,7 +6763,7 @@
         <v>2068</v>
       </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>8</v>
       </c>
@@ -6860,7 +6789,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D49">
         <v>1</v>
       </c>
@@ -6883,12 +6812,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>4</v>
       </c>
@@ -6914,7 +6843,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>8</v>
       </c>
@@ -6940,7 +6869,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
       <c r="D69">
         <v>1</v>
       </c>

</xml_diff>